<commit_message>
modified REAME.md,create the axi_bus ,append TODO-list in doc/table
</commit_message>
<xml_diff>
--- a/doc/Core/Total.xlsx
+++ b/doc/Core/Total.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27690" windowHeight="12525" activeTab="1"/>
+    <workbookView windowWidth="27690" windowHeight="12525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="参数" sheetId="1" r:id="rId1"/>
     <sheet name="存储部件数据格式" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TODOLIST" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TODOLIST!$C$1:$C$2</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>内核各参数初版决定</t>
   </si>
@@ -123,6 +126,33 @@
   </si>
   <si>
     <t>是否执行完毕</t>
+  </si>
+  <si>
+    <t>序号</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t>是否已完成</t>
+  </si>
+  <si>
+    <t>编写AXI协议SRAM接口，支持AXI3协议；
+不对axprot做要求;
+不对axcache做要求</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>编写AXI协议的空返回模块，用于返回一个为0的读事务数据</t>
+  </si>
+  <si>
+    <t>编写AXI协议的空写入模块，用于处理写事务数据;
+主要是计数aw的控制信号，并且根据协议拉高b通道的信号</t>
   </si>
 </sst>
 </file>
@@ -132,8 +162,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -159,6 +189,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -167,8 +205,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,6 +222,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -197,8 +243,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,17 +253,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,21 +268,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,24 +289,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,6 +310,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -321,13 +351,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,19 +465,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,139 +513,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,6 +578,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -559,15 +624,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,34 +646,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -626,139 +656,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -771,9 +801,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1155,145 +1191,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="7">
         <v>4</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <v>16</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>64</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>3</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="7">
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" ht="57" customHeight="1" spans="1:3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1312,7 +1348,7 @@
   <sheetPr/>
   <dimension ref="B10:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -1326,44 +1362,44 @@
   </cols>
   <sheetData>
     <row r="10" spans="2:10">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1380,14 +1416,248 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <cols>
+    <col min="2" max="2" width="44.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="81.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="66" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" ht="32" customHeight="1" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" ht="33" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+      <formula1>"IP"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+      <formula1>"IP,DEBUG,interface,spec"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
INFO: add a clk switch , add the isa exec_type,axi
</commit_message>
<xml_diff>
--- a/doc/Core/Total.xlsx
+++ b/doc/Core/Total.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27690" windowHeight="12525" activeTab="3"/>
+    <workbookView windowWidth="27690" windowHeight="12525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="参数" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
     <t>IP</t>
   </si>
   <si>
-    <t xml:space="preserve">1、目前只写了AR，R通道，AW，W，B通道还未写，未验证
+    <t xml:space="preserve">1、目前已编写完毕，未验证
 </t>
   </si>
   <si>
@@ -454,9 +454,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -470,6 +470,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -492,7 +499,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,21 +509,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -544,20 +536,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -565,9 +544,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -582,6 +560,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -590,15 +583,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,6 +600,14 @@
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -650,7 +650,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,61 +806,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,109 +830,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,11 +933,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -959,26 +976,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -987,142 +987,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1132,7 +1132,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1177,9 +1177,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1574,138 +1571,138 @@
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="21">
         <v>4</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>2</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>16</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="21"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>64</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="22">
-        <v>1</v>
-      </c>
-      <c r="C7" s="22"/>
+      <c r="B7" s="21">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>3</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="20"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="22">
-        <v>1</v>
-      </c>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="21">
+        <v>1</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>2</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" ht="57" customHeight="1" spans="1:3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1751,31 +1748,31 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1794,8 +1791,8 @@
   <sheetPr/>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1825,14 +1822,14 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1840,7 +1837,7 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1852,7 +1849,7 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2048,10 +2045,10 @@
   <sheetPr/>
   <dimension ref="A1:Y113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92:Q103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -2130,14 +2127,14 @@
       <c r="Q2" s="7">
         <v>1</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
@@ -2177,12 +2174,12 @@
       <c r="Q3" s="6">
         <v>0</v>
       </c>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
@@ -2222,12 +2219,12 @@
       <c r="Q4" s="6">
         <v>0</v>
       </c>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
@@ -2267,12 +2264,12 @@
       <c r="Q5" s="6">
         <v>0</v>
       </c>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
@@ -2569,7 +2566,7 @@
       <c r="O16" s="13"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="13"/>
-      <c r="S16" s="16"/>
+      <c r="S16" s="15"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
@@ -2609,7 +2606,7 @@
       <c r="Q17" s="7">
         <v>1</v>
       </c>
-      <c r="S17" s="17"/>
+      <c r="S17" s="16"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
@@ -2649,7 +2646,7 @@
       <c r="Q18" s="7">
         <v>1</v>
       </c>
-      <c r="S18" s="17"/>
+      <c r="S18" s="16"/>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="1" t="s">
@@ -2689,7 +2686,7 @@
       <c r="Q19" s="6">
         <v>0</v>
       </c>
-      <c r="S19" s="17"/>
+      <c r="S19" s="16"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="1" t="s">
@@ -2729,7 +2726,7 @@
       <c r="Q20" s="7">
         <v>1</v>
       </c>
-      <c r="S20" s="17"/>
+      <c r="S20" s="16"/>
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="1" t="s">
@@ -2769,7 +2766,7 @@
       <c r="Q21" s="6">
         <v>0</v>
       </c>
-      <c r="S21" s="17"/>
+      <c r="S21" s="16"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
     </row>
@@ -2811,7 +2808,7 @@
       <c r="Q22" s="6">
         <v>0</v>
       </c>
-      <c r="S22" s="17"/>
+      <c r="S22" s="16"/>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="1" t="s">
@@ -2851,7 +2848,7 @@
       <c r="Q23" s="6">
         <v>0</v>
       </c>
-      <c r="S23" s="17"/>
+      <c r="S23" s="16"/>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="1" t="s">
@@ -2891,7 +2888,7 @@
       <c r="Q24" s="7">
         <v>1</v>
       </c>
-      <c r="S24" s="17"/>
+      <c r="S24" s="16"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="1" t="s">
@@ -2929,7 +2926,7 @@
       <c r="Q25" s="10">
         <v>1</v>
       </c>
-      <c r="S25" s="17"/>
+      <c r="S25" s="16"/>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="3" t="s">
@@ -4230,7 +4227,7 @@
       <c r="Q70" s="6">
         <v>0</v>
       </c>
-      <c r="S70" s="18" t="s">
+      <c r="S70" s="17" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4270,7 +4267,7 @@
       <c r="Q71" s="6">
         <v>0</v>
       </c>
-      <c r="S71" s="18"/>
+      <c r="S71" s="17"/>
     </row>
     <row r="72" spans="1:19">
       <c r="A72" s="3" t="s">
@@ -4308,7 +4305,7 @@
       <c r="Q72" s="6">
         <v>0</v>
       </c>
-      <c r="S72" s="18"/>
+      <c r="S72" s="17"/>
     </row>
     <row r="73" spans="1:19">
       <c r="A73" s="3" t="s">
@@ -4346,7 +4343,7 @@
       <c r="Q73" s="7">
         <v>1</v>
       </c>
-      <c r="S73" s="18"/>
+      <c r="S73" s="17"/>
     </row>
     <row r="74" spans="1:19">
       <c r="A74" s="3" t="s">
@@ -4384,7 +4381,7 @@
       <c r="Q74" s="7">
         <v>1</v>
       </c>
-      <c r="S74" s="18"/>
+      <c r="S74" s="17"/>
     </row>
     <row r="75" spans="1:19">
       <c r="A75" s="3" t="s">
@@ -4422,7 +4419,7 @@
       <c r="Q75" s="7">
         <v>1</v>
       </c>
-      <c r="S75" s="18"/>
+      <c r="S75" s="17"/>
     </row>
     <row r="79" spans="14:17">
       <c r="N79" s="13" t="s">

</xml_diff>